<commit_message>
started working on proposal.
</commit_message>
<xml_diff>
--- a/proposal/timelines/flaimThesisTimelineFull.xlsx
+++ b/proposal/timelines/flaimThesisTimelineFull.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/calebflaim/Documents/thesis/openFloat/proposal/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/calebflaim/Documents/thesis/openFloat/proposal/timelines/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEC93EA5-406E-C64E-8C88-0A641043B935}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEC01A53-A8B9-9A40-B692-55878180E3DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1900" yWindow="2160" windowWidth="35840" windowHeight="21900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40" yWindow="3400" windowWidth="35840" windowHeight="21900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GanttChart" sheetId="9" r:id="rId1"/>
@@ -1557,9 +1557,6 @@
     <t>Float assembly</t>
   </si>
   <si>
-    <t>Float testing and deployment</t>
-  </si>
-  <si>
     <t>Find and order parts</t>
   </si>
   <si>
@@ -1596,9 +1593,6 @@
     <t>Learn about state machines and how to code one</t>
   </si>
   <si>
-    <t>General drifter programming</t>
-  </si>
-  <si>
     <t>General literature/youtube review for project tech components</t>
   </si>
   <si>
@@ -1689,9 +1683,6 @@
     <t>Background Research</t>
   </si>
   <si>
-    <t>Drifter testng and deployment</t>
-  </si>
-  <si>
     <t>Buoyancy engine design</t>
   </si>
   <si>
@@ -1735,6 +1726,15 @@
   </si>
   <si>
     <t>Follow ocean 444 assignment deadlines</t>
+  </si>
+  <si>
+    <t>General programming</t>
+  </si>
+  <si>
+    <t>Float testng and deployment without profiling cabability</t>
+  </si>
+  <si>
+    <t>Final float testing and deployment</t>
   </si>
 </sst>
 </file>
@@ -2713,7 +2713,7 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="164">
+  <cellXfs count="163">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3067,6 +3067,75 @@
     <xf numFmtId="0" fontId="40" fillId="25" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="50" fillId="27" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="27" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="27" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="27" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="56" fillId="29" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="29" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="27" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="45" fillId="30" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="45" fillId="27" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="45" fillId="27" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="45" fillId="27" borderId="12" xfId="40" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="51" fillId="27" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="27" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="27" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -3098,78 +3167,6 @@
     </xf>
     <xf numFmtId="0" fontId="59" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="1" fontId="50" fillId="27" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="27" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="27" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="27" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="51" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="56" fillId="29" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="29" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="27" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="45" fillId="30" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="45" fillId="27" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="45" fillId="27" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="45" fillId="27" borderId="12" xfId="40" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="51" fillId="27" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="27" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="27" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -3343,7 +3340,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$H$4" horiz="1" max="100" min="1" page="0" val="11"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$H$4" horiz="1" max="100" min="1" page="0"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4002,8 +3999,8 @@
   <dimension ref="A1:BN77"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="200" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B73" sqref="B73"/>
+      <pane ySplit="7" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4022,7 +4019,7 @@
   <sheetData>
     <row r="1" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="77" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B1" s="30"/>
       <c r="C1" s="30"/>
@@ -4030,29 +4027,29 @@
       <c r="E1" s="30"/>
       <c r="F1" s="30"/>
       <c r="I1" s="81"/>
-      <c r="K1" s="130" t="s">
+      <c r="K1" s="153" t="s">
         <v>72</v>
       </c>
-      <c r="L1" s="130"/>
-      <c r="M1" s="130"/>
-      <c r="N1" s="130"/>
-      <c r="O1" s="130"/>
-      <c r="P1" s="130"/>
-      <c r="Q1" s="130"/>
-      <c r="R1" s="130"/>
-      <c r="S1" s="130"/>
-      <c r="T1" s="130"/>
-      <c r="U1" s="130"/>
-      <c r="V1" s="130"/>
-      <c r="W1" s="130"/>
-      <c r="X1" s="130"/>
-      <c r="Y1" s="130"/>
-      <c r="Z1" s="130"/>
-      <c r="AA1" s="130"/>
-      <c r="AB1" s="130"/>
-      <c r="AC1" s="130"/>
-      <c r="AD1" s="130"/>
-      <c r="AE1" s="130"/>
+      <c r="L1" s="153"/>
+      <c r="M1" s="153"/>
+      <c r="N1" s="153"/>
+      <c r="O1" s="153"/>
+      <c r="P1" s="153"/>
+      <c r="Q1" s="153"/>
+      <c r="R1" s="153"/>
+      <c r="S1" s="153"/>
+      <c r="T1" s="153"/>
+      <c r="U1" s="153"/>
+      <c r="V1" s="153"/>
+      <c r="W1" s="153"/>
+      <c r="X1" s="153"/>
+      <c r="Y1" s="153"/>
+      <c r="Z1" s="153"/>
+      <c r="AA1" s="153"/>
+      <c r="AB1" s="153"/>
+      <c r="AC1" s="153"/>
+      <c r="AD1" s="153"/>
+      <c r="AE1" s="153"/>
     </row>
     <row r="2" spans="1:66" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="32"/>
@@ -4090,196 +4087,196 @@
       <c r="B4" s="68" t="s">
         <v>70</v>
       </c>
-      <c r="C4" s="135">
+      <c r="C4" s="158">
         <v>45196</v>
       </c>
-      <c r="D4" s="135"/>
-      <c r="E4" s="135"/>
+      <c r="D4" s="158"/>
+      <c r="E4" s="158"/>
       <c r="F4" s="67"/>
       <c r="G4" s="68" t="s">
         <v>69</v>
       </c>
       <c r="H4" s="80">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="31"/>
-      <c r="K4" s="132" t="str">
+      <c r="K4" s="155" t="str">
         <f>"Week "&amp;(K6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 11</v>
-      </c>
-      <c r="L4" s="133"/>
-      <c r="M4" s="133"/>
-      <c r="N4" s="133"/>
-      <c r="O4" s="133"/>
-      <c r="P4" s="133"/>
-      <c r="Q4" s="134"/>
-      <c r="R4" s="132" t="str">
+        <v>Week 1</v>
+      </c>
+      <c r="L4" s="156"/>
+      <c r="M4" s="156"/>
+      <c r="N4" s="156"/>
+      <c r="O4" s="156"/>
+      <c r="P4" s="156"/>
+      <c r="Q4" s="157"/>
+      <c r="R4" s="155" t="str">
         <f>"Week "&amp;(R6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 12</v>
-      </c>
-      <c r="S4" s="133"/>
-      <c r="T4" s="133"/>
-      <c r="U4" s="133"/>
-      <c r="V4" s="133"/>
-      <c r="W4" s="133"/>
-      <c r="X4" s="134"/>
-      <c r="Y4" s="132" t="str">
+        <v>Week 2</v>
+      </c>
+      <c r="S4" s="156"/>
+      <c r="T4" s="156"/>
+      <c r="U4" s="156"/>
+      <c r="V4" s="156"/>
+      <c r="W4" s="156"/>
+      <c r="X4" s="157"/>
+      <c r="Y4" s="155" t="str">
         <f>"Week "&amp;(Y6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 13</v>
-      </c>
-      <c r="Z4" s="133"/>
-      <c r="AA4" s="133"/>
-      <c r="AB4" s="133"/>
-      <c r="AC4" s="133"/>
-      <c r="AD4" s="133"/>
-      <c r="AE4" s="134"/>
-      <c r="AF4" s="132" t="str">
+        <v>Week 3</v>
+      </c>
+      <c r="Z4" s="156"/>
+      <c r="AA4" s="156"/>
+      <c r="AB4" s="156"/>
+      <c r="AC4" s="156"/>
+      <c r="AD4" s="156"/>
+      <c r="AE4" s="157"/>
+      <c r="AF4" s="155" t="str">
         <f>"Week "&amp;(AF6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 14</v>
-      </c>
-      <c r="AG4" s="133"/>
-      <c r="AH4" s="133"/>
-      <c r="AI4" s="133"/>
-      <c r="AJ4" s="133"/>
-      <c r="AK4" s="133"/>
-      <c r="AL4" s="134"/>
-      <c r="AM4" s="132" t="str">
+        <v>Week 4</v>
+      </c>
+      <c r="AG4" s="156"/>
+      <c r="AH4" s="156"/>
+      <c r="AI4" s="156"/>
+      <c r="AJ4" s="156"/>
+      <c r="AK4" s="156"/>
+      <c r="AL4" s="157"/>
+      <c r="AM4" s="155" t="str">
         <f>"Week "&amp;(AM6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 15</v>
-      </c>
-      <c r="AN4" s="133"/>
-      <c r="AO4" s="133"/>
-      <c r="AP4" s="133"/>
-      <c r="AQ4" s="133"/>
-      <c r="AR4" s="133"/>
-      <c r="AS4" s="134"/>
-      <c r="AT4" s="132" t="str">
+        <v>Week 5</v>
+      </c>
+      <c r="AN4" s="156"/>
+      <c r="AO4" s="156"/>
+      <c r="AP4" s="156"/>
+      <c r="AQ4" s="156"/>
+      <c r="AR4" s="156"/>
+      <c r="AS4" s="157"/>
+      <c r="AT4" s="155" t="str">
         <f>"Week "&amp;(AT6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 16</v>
-      </c>
-      <c r="AU4" s="133"/>
-      <c r="AV4" s="133"/>
-      <c r="AW4" s="133"/>
-      <c r="AX4" s="133"/>
-      <c r="AY4" s="133"/>
-      <c r="AZ4" s="134"/>
-      <c r="BA4" s="132" t="str">
+        <v>Week 6</v>
+      </c>
+      <c r="AU4" s="156"/>
+      <c r="AV4" s="156"/>
+      <c r="AW4" s="156"/>
+      <c r="AX4" s="156"/>
+      <c r="AY4" s="156"/>
+      <c r="AZ4" s="157"/>
+      <c r="BA4" s="155" t="str">
         <f>"Week "&amp;(BA6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 17</v>
-      </c>
-      <c r="BB4" s="133"/>
-      <c r="BC4" s="133"/>
-      <c r="BD4" s="133"/>
-      <c r="BE4" s="133"/>
-      <c r="BF4" s="133"/>
-      <c r="BG4" s="134"/>
-      <c r="BH4" s="132" t="str">
+        <v>Week 7</v>
+      </c>
+      <c r="BB4" s="156"/>
+      <c r="BC4" s="156"/>
+      <c r="BD4" s="156"/>
+      <c r="BE4" s="156"/>
+      <c r="BF4" s="156"/>
+      <c r="BG4" s="157"/>
+      <c r="BH4" s="155" t="str">
         <f>"Week "&amp;(BH6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 18</v>
-      </c>
-      <c r="BI4" s="133"/>
-      <c r="BJ4" s="133"/>
-      <c r="BK4" s="133"/>
-      <c r="BL4" s="133"/>
-      <c r="BM4" s="133"/>
-      <c r="BN4" s="134"/>
+        <v>Week 8</v>
+      </c>
+      <c r="BI4" s="156"/>
+      <c r="BJ4" s="156"/>
+      <c r="BK4" s="156"/>
+      <c r="BL4" s="156"/>
+      <c r="BM4" s="156"/>
+      <c r="BN4" s="157"/>
     </row>
     <row r="5" spans="1:66" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="67"/>
       <c r="B5" s="68" t="s">
         <v>71</v>
       </c>
-      <c r="C5" s="131" t="s">
+      <c r="C5" s="154" t="s">
         <v>131</v>
       </c>
-      <c r="D5" s="131"/>
-      <c r="E5" s="131"/>
+      <c r="D5" s="154"/>
+      <c r="E5" s="154"/>
       <c r="F5" s="67"/>
       <c r="G5" s="67"/>
       <c r="H5" s="67"/>
       <c r="I5" s="67"/>
       <c r="J5" s="31"/>
-      <c r="K5" s="136">
+      <c r="K5" s="159">
         <f>K6</f>
-        <v>45264</v>
-      </c>
-      <c r="L5" s="137"/>
-      <c r="M5" s="137"/>
-      <c r="N5" s="137"/>
-      <c r="O5" s="137"/>
-      <c r="P5" s="137"/>
-      <c r="Q5" s="138"/>
-      <c r="R5" s="136">
+        <v>45194</v>
+      </c>
+      <c r="L5" s="160"/>
+      <c r="M5" s="160"/>
+      <c r="N5" s="160"/>
+      <c r="O5" s="160"/>
+      <c r="P5" s="160"/>
+      <c r="Q5" s="161"/>
+      <c r="R5" s="159">
         <f>R6</f>
-        <v>45271</v>
-      </c>
-      <c r="S5" s="137"/>
-      <c r="T5" s="137"/>
-      <c r="U5" s="137"/>
-      <c r="V5" s="137"/>
-      <c r="W5" s="137"/>
-      <c r="X5" s="138"/>
-      <c r="Y5" s="136">
+        <v>45201</v>
+      </c>
+      <c r="S5" s="160"/>
+      <c r="T5" s="160"/>
+      <c r="U5" s="160"/>
+      <c r="V5" s="160"/>
+      <c r="W5" s="160"/>
+      <c r="X5" s="161"/>
+      <c r="Y5" s="159">
         <f>Y6</f>
-        <v>45278</v>
-      </c>
-      <c r="Z5" s="137"/>
-      <c r="AA5" s="137"/>
-      <c r="AB5" s="137"/>
-      <c r="AC5" s="137"/>
-      <c r="AD5" s="137"/>
-      <c r="AE5" s="138"/>
-      <c r="AF5" s="136">
+        <v>45208</v>
+      </c>
+      <c r="Z5" s="160"/>
+      <c r="AA5" s="160"/>
+      <c r="AB5" s="160"/>
+      <c r="AC5" s="160"/>
+      <c r="AD5" s="160"/>
+      <c r="AE5" s="161"/>
+      <c r="AF5" s="159">
         <f>AF6</f>
-        <v>45285</v>
-      </c>
-      <c r="AG5" s="137"/>
-      <c r="AH5" s="137"/>
-      <c r="AI5" s="137"/>
-      <c r="AJ5" s="137"/>
-      <c r="AK5" s="137"/>
-      <c r="AL5" s="138"/>
-      <c r="AM5" s="136">
+        <v>45215</v>
+      </c>
+      <c r="AG5" s="160"/>
+      <c r="AH5" s="160"/>
+      <c r="AI5" s="160"/>
+      <c r="AJ5" s="160"/>
+      <c r="AK5" s="160"/>
+      <c r="AL5" s="161"/>
+      <c r="AM5" s="159">
         <f>AM6</f>
-        <v>45292</v>
-      </c>
-      <c r="AN5" s="137"/>
-      <c r="AO5" s="137"/>
-      <c r="AP5" s="137"/>
-      <c r="AQ5" s="137"/>
-      <c r="AR5" s="137"/>
-      <c r="AS5" s="138"/>
-      <c r="AT5" s="136">
+        <v>45222</v>
+      </c>
+      <c r="AN5" s="160"/>
+      <c r="AO5" s="160"/>
+      <c r="AP5" s="160"/>
+      <c r="AQ5" s="160"/>
+      <c r="AR5" s="160"/>
+      <c r="AS5" s="161"/>
+      <c r="AT5" s="159">
         <f>AT6</f>
-        <v>45299</v>
-      </c>
-      <c r="AU5" s="137"/>
-      <c r="AV5" s="137"/>
-      <c r="AW5" s="137"/>
-      <c r="AX5" s="137"/>
-      <c r="AY5" s="137"/>
-      <c r="AZ5" s="138"/>
-      <c r="BA5" s="136">
+        <v>45229</v>
+      </c>
+      <c r="AU5" s="160"/>
+      <c r="AV5" s="160"/>
+      <c r="AW5" s="160"/>
+      <c r="AX5" s="160"/>
+      <c r="AY5" s="160"/>
+      <c r="AZ5" s="161"/>
+      <c r="BA5" s="159">
         <f>BA6</f>
-        <v>45306</v>
-      </c>
-      <c r="BB5" s="137"/>
-      <c r="BC5" s="137"/>
-      <c r="BD5" s="137"/>
-      <c r="BE5" s="137"/>
-      <c r="BF5" s="137"/>
-      <c r="BG5" s="138"/>
-      <c r="BH5" s="136">
+        <v>45236</v>
+      </c>
+      <c r="BB5" s="160"/>
+      <c r="BC5" s="160"/>
+      <c r="BD5" s="160"/>
+      <c r="BE5" s="160"/>
+      <c r="BF5" s="160"/>
+      <c r="BG5" s="161"/>
+      <c r="BH5" s="159">
         <f>BH6</f>
-        <v>45313</v>
-      </c>
-      <c r="BI5" s="137"/>
-      <c r="BJ5" s="137"/>
-      <c r="BK5" s="137"/>
-      <c r="BL5" s="137"/>
-      <c r="BM5" s="137"/>
-      <c r="BN5" s="138"/>
+        <v>45243</v>
+      </c>
+      <c r="BI5" s="160"/>
+      <c r="BJ5" s="160"/>
+      <c r="BK5" s="160"/>
+      <c r="BL5" s="160"/>
+      <c r="BM5" s="160"/>
+      <c r="BN5" s="161"/>
     </row>
     <row r="6" spans="1:66" x14ac:dyDescent="0.15">
       <c r="A6" s="31"/>
@@ -4294,227 +4291,227 @@
       <c r="J6" s="31"/>
       <c r="K6" s="56">
         <f>C4-WEEKDAY(C4,1)+2+7*(H4-1)</f>
-        <v>45264</v>
+        <v>45194</v>
       </c>
       <c r="L6" s="47">
         <f t="shared" ref="L6:AQ6" si="0">K6+1</f>
-        <v>45265</v>
+        <v>45195</v>
       </c>
       <c r="M6" s="47">
         <f t="shared" si="0"/>
-        <v>45266</v>
+        <v>45196</v>
       </c>
       <c r="N6" s="47">
         <f t="shared" si="0"/>
-        <v>45267</v>
+        <v>45197</v>
       </c>
       <c r="O6" s="47">
         <f t="shared" si="0"/>
-        <v>45268</v>
+        <v>45198</v>
       </c>
       <c r="P6" s="47">
         <f t="shared" si="0"/>
-        <v>45269</v>
+        <v>45199</v>
       </c>
       <c r="Q6" s="57">
         <f t="shared" si="0"/>
-        <v>45270</v>
+        <v>45200</v>
       </c>
       <c r="R6" s="56">
         <f t="shared" si="0"/>
-        <v>45271</v>
+        <v>45201</v>
       </c>
       <c r="S6" s="47">
         <f t="shared" si="0"/>
-        <v>45272</v>
+        <v>45202</v>
       </c>
       <c r="T6" s="47">
         <f t="shared" si="0"/>
-        <v>45273</v>
+        <v>45203</v>
       </c>
       <c r="U6" s="47">
         <f t="shared" si="0"/>
-        <v>45274</v>
+        <v>45204</v>
       </c>
       <c r="V6" s="47">
         <f t="shared" si="0"/>
-        <v>45275</v>
+        <v>45205</v>
       </c>
       <c r="W6" s="47">
         <f t="shared" si="0"/>
-        <v>45276</v>
+        <v>45206</v>
       </c>
       <c r="X6" s="57">
         <f t="shared" si="0"/>
-        <v>45277</v>
+        <v>45207</v>
       </c>
       <c r="Y6" s="56">
         <f t="shared" si="0"/>
-        <v>45278</v>
+        <v>45208</v>
       </c>
       <c r="Z6" s="47">
         <f t="shared" si="0"/>
-        <v>45279</v>
+        <v>45209</v>
       </c>
       <c r="AA6" s="47">
         <f t="shared" si="0"/>
-        <v>45280</v>
+        <v>45210</v>
       </c>
       <c r="AB6" s="47">
         <f t="shared" si="0"/>
-        <v>45281</v>
+        <v>45211</v>
       </c>
       <c r="AC6" s="47">
         <f t="shared" si="0"/>
-        <v>45282</v>
+        <v>45212</v>
       </c>
       <c r="AD6" s="47">
         <f t="shared" si="0"/>
-        <v>45283</v>
+        <v>45213</v>
       </c>
       <c r="AE6" s="57">
         <f t="shared" si="0"/>
-        <v>45284</v>
+        <v>45214</v>
       </c>
       <c r="AF6" s="56">
         <f t="shared" si="0"/>
-        <v>45285</v>
+        <v>45215</v>
       </c>
       <c r="AG6" s="47">
         <f t="shared" si="0"/>
-        <v>45286</v>
+        <v>45216</v>
       </c>
       <c r="AH6" s="47">
         <f t="shared" si="0"/>
-        <v>45287</v>
+        <v>45217</v>
       </c>
       <c r="AI6" s="47">
         <f t="shared" si="0"/>
-        <v>45288</v>
+        <v>45218</v>
       </c>
       <c r="AJ6" s="47">
         <f t="shared" si="0"/>
-        <v>45289</v>
+        <v>45219</v>
       </c>
       <c r="AK6" s="47">
         <f t="shared" si="0"/>
-        <v>45290</v>
+        <v>45220</v>
       </c>
       <c r="AL6" s="57">
         <f t="shared" si="0"/>
-        <v>45291</v>
+        <v>45221</v>
       </c>
       <c r="AM6" s="56">
         <f t="shared" si="0"/>
-        <v>45292</v>
+        <v>45222</v>
       </c>
       <c r="AN6" s="47">
         <f t="shared" si="0"/>
-        <v>45293</v>
+        <v>45223</v>
       </c>
       <c r="AO6" s="47">
         <f t="shared" si="0"/>
-        <v>45294</v>
+        <v>45224</v>
       </c>
       <c r="AP6" s="47">
         <f t="shared" si="0"/>
-        <v>45295</v>
+        <v>45225</v>
       </c>
       <c r="AQ6" s="47">
         <f t="shared" si="0"/>
-        <v>45296</v>
+        <v>45226</v>
       </c>
       <c r="AR6" s="47">
         <f t="shared" ref="AR6:BN6" si="1">AQ6+1</f>
-        <v>45297</v>
+        <v>45227</v>
       </c>
       <c r="AS6" s="57">
         <f t="shared" si="1"/>
-        <v>45298</v>
+        <v>45228</v>
       </c>
       <c r="AT6" s="56">
         <f t="shared" si="1"/>
-        <v>45299</v>
+        <v>45229</v>
       </c>
       <c r="AU6" s="47">
         <f t="shared" si="1"/>
-        <v>45300</v>
+        <v>45230</v>
       </c>
       <c r="AV6" s="47">
         <f t="shared" si="1"/>
-        <v>45301</v>
+        <v>45231</v>
       </c>
       <c r="AW6" s="47">
         <f t="shared" si="1"/>
-        <v>45302</v>
+        <v>45232</v>
       </c>
       <c r="AX6" s="47">
         <f t="shared" si="1"/>
-        <v>45303</v>
+        <v>45233</v>
       </c>
       <c r="AY6" s="47">
         <f t="shared" si="1"/>
-        <v>45304</v>
+        <v>45234</v>
       </c>
       <c r="AZ6" s="57">
         <f t="shared" si="1"/>
-        <v>45305</v>
+        <v>45235</v>
       </c>
       <c r="BA6" s="56">
         <f t="shared" si="1"/>
-        <v>45306</v>
+        <v>45236</v>
       </c>
       <c r="BB6" s="47">
         <f t="shared" si="1"/>
-        <v>45307</v>
+        <v>45237</v>
       </c>
       <c r="BC6" s="47">
         <f t="shared" si="1"/>
-        <v>45308</v>
+        <v>45238</v>
       </c>
       <c r="BD6" s="47">
         <f t="shared" si="1"/>
-        <v>45309</v>
+        <v>45239</v>
       </c>
       <c r="BE6" s="47">
         <f t="shared" si="1"/>
-        <v>45310</v>
+        <v>45240</v>
       </c>
       <c r="BF6" s="47">
         <f t="shared" si="1"/>
-        <v>45311</v>
+        <v>45241</v>
       </c>
       <c r="BG6" s="57">
         <f t="shared" si="1"/>
-        <v>45312</v>
+        <v>45242</v>
       </c>
       <c r="BH6" s="56">
         <f t="shared" si="1"/>
-        <v>45313</v>
+        <v>45243</v>
       </c>
       <c r="BI6" s="47">
         <f t="shared" si="1"/>
-        <v>45314</v>
+        <v>45244</v>
       </c>
       <c r="BJ6" s="47">
         <f t="shared" si="1"/>
-        <v>45315</v>
+        <v>45245</v>
       </c>
       <c r="BK6" s="47">
         <f t="shared" si="1"/>
-        <v>45316</v>
+        <v>45246</v>
       </c>
       <c r="BL6" s="47">
         <f t="shared" si="1"/>
-        <v>45317</v>
+        <v>45247</v>
       </c>
       <c r="BM6" s="47">
         <f t="shared" si="1"/>
-        <v>45318</v>
+        <v>45248</v>
       </c>
       <c r="BN6" s="57">
         <f t="shared" si="1"/>
-        <v>45319</v>
+        <v>45249</v>
       </c>
     </row>
     <row r="7" spans="1:66" s="2" customFormat="1" ht="27" thickBot="1" x14ac:dyDescent="0.2">
@@ -4777,7 +4774,7 @@
         <v>1</v>
       </c>
       <c r="B8" s="49" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C8" s="50"/>
       <c r="D8" s="51"/>
@@ -4943,7 +4940,7 @@
         <v>1.1.1</v>
       </c>
       <c r="B10" s="78" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D10" s="79"/>
       <c r="E10" s="61"/>
@@ -5015,7 +5012,7 @@
         <v>1.1.2</v>
       </c>
       <c r="B11" s="78" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D11" s="79"/>
       <c r="E11" s="61">
@@ -5099,7 +5096,7 @@
         <v>1.1.3</v>
       </c>
       <c r="B12" s="41" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D12" s="79"/>
       <c r="E12" s="61">
@@ -5183,7 +5180,7 @@
         <v>1.1.4</v>
       </c>
       <c r="B13" s="78" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D13" s="79"/>
       <c r="E13" s="61">
@@ -5267,7 +5264,7 @@
         <v>1.2</v>
       </c>
       <c r="B14" s="120" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C14" s="121"/>
       <c r="D14" s="122"/>
@@ -5340,7 +5337,7 @@
         <v>1.2.1</v>
       </c>
       <c r="B15" s="78" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C15" s="109"/>
       <c r="D15" s="110"/>
@@ -5425,7 +5422,7 @@
         <v>1.2.2</v>
       </c>
       <c r="B16" s="78" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C16" s="109"/>
       <c r="D16" s="110"/>
@@ -5510,7 +5507,7 @@
         <v>1.2.3</v>
       </c>
       <c r="B17" s="78" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C17" s="109"/>
       <c r="D17" s="110"/>
@@ -5595,7 +5592,7 @@
         <v>1.3</v>
       </c>
       <c r="B18" s="129" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C18" s="121"/>
       <c r="D18" s="122"/>
@@ -5668,7 +5665,7 @@
         <v>1.3.1</v>
       </c>
       <c r="B19" s="78" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D19" s="79"/>
       <c r="E19" s="61">
@@ -5752,7 +5749,7 @@
         <v>1.3.2</v>
       </c>
       <c r="B20" s="78" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D20" s="79"/>
       <c r="E20" s="61">
@@ -5836,7 +5833,7 @@
         <v>1.3.3</v>
       </c>
       <c r="B21" s="78" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D21" s="79"/>
       <c r="E21" s="61">
@@ -5920,7 +5917,7 @@
         <v>1.3.4</v>
       </c>
       <c r="B22" s="78" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D22" s="79"/>
       <c r="E22" s="61">
@@ -6004,7 +6001,7 @@
         <v>1.3.5</v>
       </c>
       <c r="B23" s="78" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D23" s="79"/>
       <c r="E23" s="61">
@@ -6161,7 +6158,7 @@
         <v>1.4.1</v>
       </c>
       <c r="B25" s="78" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D25" s="79"/>
       <c r="E25" s="61">
@@ -6245,7 +6242,7 @@
         <v>1.4.2</v>
       </c>
       <c r="B26" s="41" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D26" s="79"/>
       <c r="E26" s="61">
@@ -6329,7 +6326,7 @@
         <v>1.4.3</v>
       </c>
       <c r="B27" s="78" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D27" s="79"/>
       <c r="E27" s="61">
@@ -6485,7 +6482,7 @@
         <v>1.5.1</v>
       </c>
       <c r="B29" s="78" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D29" s="79"/>
       <c r="E29" s="61">
@@ -6569,7 +6566,7 @@
         <v>1.5.2</v>
       </c>
       <c r="B30" s="78" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D30" s="79"/>
       <c r="E30" s="61">
@@ -6653,7 +6650,7 @@
         <v>1.5.3</v>
       </c>
       <c r="B31" s="78" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D31" s="79"/>
       <c r="E31" s="61">
@@ -6737,7 +6734,7 @@
         <v>1.5.4</v>
       </c>
       <c r="B32" s="78" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D32" s="79"/>
       <c r="E32" s="61">
@@ -6815,13 +6812,13 @@
       <c r="BM32" s="108"/>
       <c r="BN32" s="108"/>
     </row>
-    <row r="33" spans="1:66" s="113" customFormat="1" ht="26" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:66" s="113" customFormat="1" ht="18" x14ac:dyDescent="0.15">
       <c r="A33" s="112" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>1.6</v>
       </c>
       <c r="B33" s="129" t="s">
-        <v>149</v>
+        <v>193</v>
       </c>
       <c r="D33" s="122"/>
       <c r="E33" s="123"/>
@@ -6893,7 +6890,7 @@
         <v>1.6.1</v>
       </c>
       <c r="B34" s="78" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D34" s="79"/>
       <c r="E34" s="61">
@@ -6977,7 +6974,7 @@
         <v>1.6.2</v>
       </c>
       <c r="B35" s="78" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D35" s="79"/>
       <c r="E35" s="61">
@@ -7061,7 +7058,7 @@
         <v>1.6.3</v>
       </c>
       <c r="B36" s="78" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D36" s="79"/>
       <c r="E36" s="61">
@@ -7139,13 +7136,13 @@
       <c r="BM36" s="108"/>
       <c r="BN36" s="108"/>
     </row>
-    <row r="37" spans="1:66" s="113" customFormat="1" ht="26" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:66" s="113" customFormat="1" ht="39" x14ac:dyDescent="0.15">
       <c r="A37" s="112" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>1.7</v>
       </c>
       <c r="B37" s="129" t="s">
-        <v>180</v>
+        <v>194</v>
       </c>
       <c r="D37" s="122"/>
       <c r="E37" s="123"/>
@@ -7217,7 +7214,7 @@
         <v>1.7.1</v>
       </c>
       <c r="B38" s="78" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D38" s="79"/>
       <c r="E38" s="61">
@@ -7301,7 +7298,7 @@
         <v>1.7.2</v>
       </c>
       <c r="B39" s="78" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D39" s="79"/>
       <c r="E39" s="61">
@@ -7385,7 +7382,7 @@
         <v>1.7.3</v>
       </c>
       <c r="B40" s="78" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D40" s="79"/>
       <c r="E40" s="61">
@@ -7469,7 +7466,7 @@
         <v>1.8</v>
       </c>
       <c r="B41" s="129" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="D41" s="122"/>
       <c r="E41" s="123"/>
@@ -7541,7 +7538,7 @@
         <v>1.8.1</v>
       </c>
       <c r="B42" s="78" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D42" s="79"/>
       <c r="E42" s="61">
@@ -7625,7 +7622,7 @@
         <v>1.8.2</v>
       </c>
       <c r="B43" s="78" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D43" s="79"/>
       <c r="E43" s="61">
@@ -7709,7 +7706,7 @@
         <v>1.8.3</v>
       </c>
       <c r="B44" s="78" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D44" s="79"/>
       <c r="E44" s="61">
@@ -7793,7 +7790,7 @@
         <v>1.9</v>
       </c>
       <c r="B45" s="129" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D45" s="122"/>
       <c r="E45" s="123"/>
@@ -7865,7 +7862,7 @@
         <v>1.9.1</v>
       </c>
       <c r="B46" s="78" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D46" s="79"/>
       <c r="E46" s="61">
@@ -7949,7 +7946,7 @@
         <v>1.9.2</v>
       </c>
       <c r="B47" s="78" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D47" s="79"/>
       <c r="E47" s="61">
@@ -8033,7 +8030,7 @@
         <v>1.9.3</v>
       </c>
       <c r="B48" s="78" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D48" s="79"/>
       <c r="E48" s="61">
@@ -8117,7 +8114,7 @@
         <v>1.9.4</v>
       </c>
       <c r="B49" s="78" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D49" s="79"/>
       <c r="E49" s="61">
@@ -8273,7 +8270,7 @@
         <v>1.10.1</v>
       </c>
       <c r="B51" s="78" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D51" s="79"/>
       <c r="E51" s="61">
@@ -8357,7 +8354,7 @@
         <v>1.10.2</v>
       </c>
       <c r="B52" s="78" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D52" s="79"/>
       <c r="E52" s="61">
@@ -8441,7 +8438,7 @@
         <v>1.10.3</v>
       </c>
       <c r="B53" s="78" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D53" s="79"/>
       <c r="E53" s="61">
@@ -8525,7 +8522,7 @@
         <v>1.11</v>
       </c>
       <c r="B54" s="129" t="s">
-        <v>136</v>
+        <v>195</v>
       </c>
       <c r="D54" s="122"/>
       <c r="E54" s="123"/>
@@ -8597,7 +8594,7 @@
         <v>1.12</v>
       </c>
       <c r="B55" s="78" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D55" s="79"/>
       <c r="E55" s="61">
@@ -8681,7 +8678,7 @@
         <v>1.12.1</v>
       </c>
       <c r="B56" s="78" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D56" s="79"/>
       <c r="E56" s="61">
@@ -8765,7 +8762,7 @@
         <v>1.13</v>
       </c>
       <c r="B57" s="78" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D57" s="79"/>
       <c r="E57" s="61">
@@ -8849,7 +8846,7 @@
         <v>2</v>
       </c>
       <c r="B58" s="34" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="D58" s="36"/>
       <c r="E58" s="63"/>
@@ -8921,13 +8918,13 @@
       <c r="BM58" s="66"/>
       <c r="BN58" s="66"/>
     </row>
-    <row r="59" spans="1:66" s="143" customFormat="1" ht="18" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:66" s="133" customFormat="1" ht="18" x14ac:dyDescent="0.15">
       <c r="A59" s="40" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>2.1</v>
       </c>
       <c r="B59" s="78" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C59" s="41"/>
       <c r="D59" s="79"/>
@@ -8948,63 +8945,63 @@
         <f t="shared" si="28"/>
         <v>16</v>
       </c>
-      <c r="J59" s="140"/>
-      <c r="K59" s="141"/>
-      <c r="L59" s="141"/>
-      <c r="M59" s="141"/>
-      <c r="N59" s="141"/>
-      <c r="O59" s="141"/>
-      <c r="P59" s="141"/>
-      <c r="Q59" s="141"/>
-      <c r="R59" s="141"/>
-      <c r="S59" s="141"/>
-      <c r="T59" s="141"/>
-      <c r="U59" s="141"/>
-      <c r="V59" s="141"/>
-      <c r="W59" s="141"/>
-      <c r="X59" s="141"/>
-      <c r="Y59" s="141"/>
-      <c r="Z59" s="141"/>
-      <c r="AA59" s="141"/>
-      <c r="AB59" s="141"/>
-      <c r="AC59" s="141"/>
-      <c r="AD59" s="141"/>
-      <c r="AE59" s="141"/>
-      <c r="AF59" s="141"/>
-      <c r="AG59" s="141"/>
-      <c r="AH59" s="141"/>
-      <c r="AI59" s="141"/>
-      <c r="AJ59" s="141"/>
-      <c r="AK59" s="141"/>
-      <c r="AL59" s="141"/>
-      <c r="AM59" s="141"/>
-      <c r="AN59" s="141"/>
-      <c r="AO59" s="141"/>
-      <c r="AP59" s="141"/>
-      <c r="AQ59" s="141"/>
-      <c r="AR59" s="141"/>
-      <c r="AS59" s="141"/>
-      <c r="AT59" s="141"/>
-      <c r="AU59" s="141"/>
-      <c r="AV59" s="141"/>
-      <c r="AW59" s="141"/>
-      <c r="AX59" s="141"/>
-      <c r="AY59" s="141"/>
-      <c r="AZ59" s="141"/>
-      <c r="BA59" s="141"/>
-      <c r="BB59" s="141"/>
-      <c r="BC59" s="141"/>
-      <c r="BD59" s="141"/>
-      <c r="BE59" s="141"/>
-      <c r="BF59" s="141"/>
-      <c r="BG59" s="141"/>
-      <c r="BH59" s="141"/>
-      <c r="BI59" s="141"/>
-      <c r="BJ59" s="141"/>
-      <c r="BK59" s="141"/>
-      <c r="BL59" s="141"/>
-      <c r="BM59" s="141"/>
-      <c r="BN59" s="141"/>
+      <c r="J59" s="130"/>
+      <c r="K59" s="131"/>
+      <c r="L59" s="131"/>
+      <c r="M59" s="131"/>
+      <c r="N59" s="131"/>
+      <c r="O59" s="131"/>
+      <c r="P59" s="131"/>
+      <c r="Q59" s="131"/>
+      <c r="R59" s="131"/>
+      <c r="S59" s="131"/>
+      <c r="T59" s="131"/>
+      <c r="U59" s="131"/>
+      <c r="V59" s="131"/>
+      <c r="W59" s="131"/>
+      <c r="X59" s="131"/>
+      <c r="Y59" s="131"/>
+      <c r="Z59" s="131"/>
+      <c r="AA59" s="131"/>
+      <c r="AB59" s="131"/>
+      <c r="AC59" s="131"/>
+      <c r="AD59" s="131"/>
+      <c r="AE59" s="131"/>
+      <c r="AF59" s="131"/>
+      <c r="AG59" s="131"/>
+      <c r="AH59" s="131"/>
+      <c r="AI59" s="131"/>
+      <c r="AJ59" s="131"/>
+      <c r="AK59" s="131"/>
+      <c r="AL59" s="131"/>
+      <c r="AM59" s="131"/>
+      <c r="AN59" s="131"/>
+      <c r="AO59" s="131"/>
+      <c r="AP59" s="131"/>
+      <c r="AQ59" s="131"/>
+      <c r="AR59" s="131"/>
+      <c r="AS59" s="131"/>
+      <c r="AT59" s="131"/>
+      <c r="AU59" s="131"/>
+      <c r="AV59" s="131"/>
+      <c r="AW59" s="131"/>
+      <c r="AX59" s="131"/>
+      <c r="AY59" s="131"/>
+      <c r="AZ59" s="131"/>
+      <c r="BA59" s="131"/>
+      <c r="BB59" s="131"/>
+      <c r="BC59" s="131"/>
+      <c r="BD59" s="131"/>
+      <c r="BE59" s="131"/>
+      <c r="BF59" s="131"/>
+      <c r="BG59" s="131"/>
+      <c r="BH59" s="131"/>
+      <c r="BI59" s="131"/>
+      <c r="BJ59" s="131"/>
+      <c r="BK59" s="131"/>
+      <c r="BL59" s="131"/>
+      <c r="BM59" s="131"/>
+      <c r="BN59" s="131"/>
     </row>
     <row r="60" spans="1:66" s="35" customFormat="1" ht="18" x14ac:dyDescent="0.15">
       <c r="A60" s="33" t="str">
@@ -9012,7 +9009,7 @@
         <v>3</v>
       </c>
       <c r="B60" s="34" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D60" s="36"/>
       <c r="E60" s="63"/>
@@ -9090,7 +9087,7 @@
         <v>3.1</v>
       </c>
       <c r="B61" s="78" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="D61" s="79"/>
       <c r="E61" s="61">
@@ -9174,7 +9171,7 @@
         <v>3.2</v>
       </c>
       <c r="B62" s="78" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="D62" s="79"/>
       <c r="E62" s="61">
@@ -9258,7 +9255,7 @@
         <v>3.3</v>
       </c>
       <c r="B63" s="78" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="D63" s="79"/>
       <c r="E63" s="61">
@@ -9342,7 +9339,7 @@
         <v>3.4</v>
       </c>
       <c r="B64" s="78" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="D64" s="79"/>
       <c r="E64" s="61">
@@ -9426,7 +9423,7 @@
         <v>3.4.1</v>
       </c>
       <c r="B65" s="78" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D65" s="79"/>
       <c r="E65" s="61">
@@ -9510,7 +9507,7 @@
         <v>3.5</v>
       </c>
       <c r="B66" s="78" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="D66" s="79"/>
       <c r="E66" s="61">
@@ -9594,7 +9591,7 @@
         <v>3.6</v>
       </c>
       <c r="B67" s="78" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="D67" s="79"/>
       <c r="E67" s="61">
@@ -9614,7 +9611,7 @@
         <f t="shared" ref="I67" si="35">IF(OR(F67=0,E67=0)," - ",NETWORKDAYS(E67,F67))</f>
         <v>3</v>
       </c>
-      <c r="J67" s="144"/>
+      <c r="J67" s="111"/>
       <c r="K67" s="40"/>
       <c r="L67" s="40"/>
       <c r="M67" s="40"/>
@@ -9678,7 +9675,7 @@
         <v>3.7</v>
       </c>
       <c r="B68" s="78" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="D68" s="79"/>
       <c r="E68" s="61">
@@ -9698,7 +9695,7 @@
         <f t="shared" ref="I68" si="37">IF(OR(F68=0,E68=0)," - ",NETWORKDAYS(E68,F68))</f>
         <v>3</v>
       </c>
-      <c r="J68" s="144"/>
+      <c r="J68" s="111"/>
       <c r="K68" s="40"/>
       <c r="L68" s="40"/>
       <c r="M68" s="40"/>
@@ -9762,7 +9759,7 @@
         <v>4</v>
       </c>
       <c r="B69" s="34" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D69" s="36"/>
       <c r="E69" s="63"/>
@@ -9840,7 +9837,7 @@
         <v>4.1</v>
       </c>
       <c r="B70" s="78" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D70" s="79"/>
       <c r="E70" s="61">
@@ -9919,17 +9916,17 @@
       <c r="BN70" s="40"/>
     </row>
     <row r="71" spans="1:66" s="46" customFormat="1" ht="18" x14ac:dyDescent="0.15">
-      <c r="A71" s="145"/>
-      <c r="B71" s="146"/>
-      <c r="C71" s="147"/>
-      <c r="D71" s="147"/>
-      <c r="E71" s="148"/>
-      <c r="F71" s="148"/>
-      <c r="G71" s="149"/>
-      <c r="H71" s="149"/>
-      <c r="I71" s="149"/>
-      <c r="J71" s="150"/>
-      <c r="K71" s="141"/>
+      <c r="A71" s="134"/>
+      <c r="B71" s="135"/>
+      <c r="C71" s="136"/>
+      <c r="D71" s="136"/>
+      <c r="E71" s="137"/>
+      <c r="F71" s="137"/>
+      <c r="G71" s="138"/>
+      <c r="H71" s="138"/>
+      <c r="I71" s="138"/>
+      <c r="J71" s="139"/>
+      <c r="K71" s="131"/>
       <c r="L71" s="40"/>
       <c r="M71" s="40"/>
       <c r="N71" s="40"/>
@@ -9987,17 +9984,17 @@
       <c r="BN71" s="40"/>
     </row>
     <row r="72" spans="1:66" s="45" customFormat="1" ht="18" x14ac:dyDescent="0.15">
-      <c r="A72" s="151"/>
-      <c r="B72" s="152"/>
-      <c r="C72" s="152"/>
-      <c r="D72" s="152"/>
-      <c r="E72" s="153"/>
-      <c r="F72" s="153"/>
-      <c r="G72" s="152"/>
-      <c r="H72" s="152"/>
-      <c r="I72" s="152"/>
-      <c r="J72" s="150"/>
-      <c r="K72" s="141"/>
+      <c r="A72" s="140"/>
+      <c r="B72" s="141"/>
+      <c r="C72" s="141"/>
+      <c r="D72" s="141"/>
+      <c r="E72" s="142"/>
+      <c r="F72" s="142"/>
+      <c r="G72" s="141"/>
+      <c r="H72" s="141"/>
+      <c r="I72" s="141"/>
+      <c r="J72" s="139"/>
+      <c r="K72" s="131"/>
       <c r="L72" s="40"/>
       <c r="M72" s="40"/>
       <c r="N72" s="40"/>
@@ -10055,17 +10052,17 @@
       <c r="BN72" s="40"/>
     </row>
     <row r="73" spans="1:66" s="45" customFormat="1" ht="18" x14ac:dyDescent="0.15">
-      <c r="A73" s="142"/>
-      <c r="B73" s="154"/>
-      <c r="C73" s="155"/>
-      <c r="D73" s="156"/>
-      <c r="E73" s="157"/>
-      <c r="F73" s="158"/>
-      <c r="G73" s="159"/>
-      <c r="H73" s="160"/>
-      <c r="I73" s="159"/>
-      <c r="J73" s="161"/>
-      <c r="K73" s="141"/>
+      <c r="A73" s="132"/>
+      <c r="B73" s="143"/>
+      <c r="C73" s="144"/>
+      <c r="D73" s="145"/>
+      <c r="E73" s="146"/>
+      <c r="F73" s="147"/>
+      <c r="G73" s="148"/>
+      <c r="H73" s="149"/>
+      <c r="I73" s="148"/>
+      <c r="J73" s="150"/>
+      <c r="K73" s="131"/>
       <c r="L73" s="40"/>
       <c r="M73" s="40"/>
       <c r="N73" s="40"/>
@@ -10123,17 +10120,17 @@
       <c r="BN73" s="40"/>
     </row>
     <row r="74" spans="1:66" s="45" customFormat="1" ht="18" x14ac:dyDescent="0.15">
-      <c r="A74" s="141"/>
-      <c r="B74" s="162"/>
-      <c r="C74" s="162"/>
-      <c r="D74" s="156"/>
-      <c r="E74" s="157"/>
-      <c r="F74" s="158"/>
-      <c r="G74" s="159"/>
-      <c r="H74" s="160"/>
-      <c r="I74" s="159"/>
-      <c r="J74" s="161"/>
-      <c r="K74" s="141"/>
+      <c r="A74" s="131"/>
+      <c r="B74" s="151"/>
+      <c r="C74" s="151"/>
+      <c r="D74" s="145"/>
+      <c r="E74" s="146"/>
+      <c r="F74" s="147"/>
+      <c r="G74" s="148"/>
+      <c r="H74" s="149"/>
+      <c r="I74" s="148"/>
+      <c r="J74" s="150"/>
+      <c r="K74" s="131"/>
       <c r="L74" s="40"/>
       <c r="M74" s="40"/>
       <c r="N74" s="40"/>
@@ -10191,17 +10188,17 @@
       <c r="BN74" s="40"/>
     </row>
     <row r="75" spans="1:66" s="45" customFormat="1" ht="18" x14ac:dyDescent="0.15">
-      <c r="A75" s="141"/>
-      <c r="B75" s="163"/>
-      <c r="C75" s="162"/>
-      <c r="D75" s="156"/>
-      <c r="E75" s="157"/>
-      <c r="F75" s="158"/>
-      <c r="G75" s="159"/>
-      <c r="H75" s="160"/>
-      <c r="I75" s="159"/>
-      <c r="J75" s="161"/>
-      <c r="K75" s="141"/>
+      <c r="A75" s="131"/>
+      <c r="B75" s="152"/>
+      <c r="C75" s="151"/>
+      <c r="D75" s="145"/>
+      <c r="E75" s="146"/>
+      <c r="F75" s="147"/>
+      <c r="G75" s="148"/>
+      <c r="H75" s="149"/>
+      <c r="I75" s="148"/>
+      <c r="J75" s="150"/>
+      <c r="K75" s="131"/>
       <c r="L75" s="40"/>
       <c r="M75" s="40"/>
       <c r="N75" s="40"/>
@@ -10259,17 +10256,17 @@
       <c r="BN75" s="40"/>
     </row>
     <row r="76" spans="1:66" s="45" customFormat="1" ht="18" x14ac:dyDescent="0.15">
-      <c r="A76" s="141"/>
-      <c r="B76" s="163"/>
-      <c r="C76" s="162"/>
-      <c r="D76" s="156"/>
-      <c r="E76" s="157"/>
-      <c r="F76" s="158"/>
-      <c r="G76" s="159"/>
-      <c r="H76" s="160"/>
-      <c r="I76" s="159"/>
-      <c r="J76" s="161"/>
-      <c r="K76" s="141"/>
+      <c r="A76" s="131"/>
+      <c r="B76" s="152"/>
+      <c r="C76" s="151"/>
+      <c r="D76" s="145"/>
+      <c r="E76" s="146"/>
+      <c r="F76" s="147"/>
+      <c r="G76" s="148"/>
+      <c r="H76" s="149"/>
+      <c r="I76" s="148"/>
+      <c r="J76" s="150"/>
+      <c r="K76" s="131"/>
       <c r="L76" s="40"/>
       <c r="M76" s="40"/>
       <c r="N76" s="40"/>
@@ -10703,10 +10700,10 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A13" s="139" t="s">
+      <c r="A13" s="162" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="139"/>
+      <c r="B13" s="162"/>
     </row>
     <row r="15" spans="1:3" s="83" customFormat="1" ht="18" x14ac:dyDescent="0.15">
       <c r="A15" s="90"/>
@@ -10767,10 +10764,10 @@
       <c r="B23" s="4"/>
     </row>
     <row r="24" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A24" s="139" t="s">
+      <c r="A24" s="162" t="s">
         <v>80</v>
       </c>
-      <c r="B24" s="139"/>
+      <c r="B24" s="162"/>
     </row>
     <row r="25" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A25" s="91"/>
@@ -10843,10 +10840,10 @@
       <c r="B37" s="4"/>
     </row>
     <row r="38" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A38" s="139" t="s">
+      <c r="A38" s="162" t="s">
         <v>9</v>
       </c>
-      <c r="B38" s="139"/>
+      <c r="B38" s="162"/>
     </row>
     <row r="39" spans="1:2" ht="30" x14ac:dyDescent="0.15">
       <c r="B39" s="89" t="s">
@@ -10877,10 +10874,10 @@
       </c>
     </row>
     <row r="49" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A49" s="139" t="s">
+      <c r="A49" s="162" t="s">
         <v>6</v>
       </c>
-      <c r="B49" s="139"/>
+      <c r="B49" s="162"/>
     </row>
     <row r="50" spans="1:2" ht="30" x14ac:dyDescent="0.15">
       <c r="B50" s="89" t="s">
@@ -10975,10 +10972,10 @@
       <c r="B64" s="5"/>
     </row>
     <row r="65" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A65" s="139" t="s">
+      <c r="A65" s="162" t="s">
         <v>8</v>
       </c>
-      <c r="B65" s="139"/>
+      <c r="B65" s="162"/>
     </row>
     <row r="66" spans="1:2" ht="45" x14ac:dyDescent="0.15">
       <c r="B66" s="89" t="s">
@@ -10986,10 +10983,10 @@
       </c>
     </row>
     <row r="68" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A68" s="139" t="s">
+      <c r="A68" s="162" t="s">
         <v>4</v>
       </c>
-      <c r="B68" s="139"/>
+      <c r="B68" s="162"/>
     </row>
     <row r="69" spans="1:2" ht="15" x14ac:dyDescent="0.15">
       <c r="A69" s="101" t="s">

</xml_diff>

<commit_message>
Updated timeline and made a budget
</commit_message>
<xml_diff>
--- a/proposal/timelines/flaimThesisTimelineFull.xlsx
+++ b/proposal/timelines/flaimThesisTimelineFull.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/calebflaim/Documents/thesis/openFloat/proposal/timelines/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEC01A53-A8B9-9A40-B692-55878180E3DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DA59420-7F8B-7C43-916B-1135A404F082}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40" yWindow="3400" windowWidth="35840" windowHeight="21900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GanttChart" sheetId="9" r:id="rId1"/>
@@ -1659,15 +1659,9 @@
     <t>Overnight tests in test tank</t>
   </si>
   <si>
-    <t>Deployment</t>
-  </si>
-  <si>
     <t>Ensure float can, at a minimum, broadcast GPS position over radio</t>
   </si>
   <si>
-    <t>Deply drifter with SSC</t>
-  </si>
-  <si>
     <t>Meet with Trevor to finalize design</t>
   </si>
   <si>
@@ -1677,9 +1671,6 @@
     <t>openFloat V1 Project Schedule</t>
   </si>
   <si>
-    <t>Float Building Stage</t>
-  </si>
-  <si>
     <t>Background Research</t>
   </si>
   <si>
@@ -1735,6 +1726,15 @@
   </si>
   <si>
     <t>Final float testing and deployment</t>
+  </si>
+  <si>
+    <t>Deployment in Colvos Passage</t>
+  </si>
+  <si>
+    <t>Deploy float prototype near Shillshole</t>
+  </si>
+  <si>
+    <t>Float Devolpment Stage</t>
   </si>
 </sst>
 </file>
@@ -3999,8 +3999,8 @@
   <dimension ref="A1:BN77"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="200" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B66" sqref="B66"/>
+      <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4019,7 +4019,7 @@
   <sheetData>
     <row r="1" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="77" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B1" s="30"/>
       <c r="C1" s="30"/>
@@ -4774,7 +4774,7 @@
         <v>1</v>
       </c>
       <c r="B8" s="49" t="s">
-        <v>176</v>
+        <v>195</v>
       </c>
       <c r="C8" s="50"/>
       <c r="D8" s="51"/>
@@ -5592,7 +5592,7 @@
         <v>1.3</v>
       </c>
       <c r="B18" s="129" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C18" s="121"/>
       <c r="D18" s="122"/>
@@ -6818,7 +6818,7 @@
         <v>1.6</v>
       </c>
       <c r="B33" s="129" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="D33" s="122"/>
       <c r="E33" s="123"/>
@@ -7142,7 +7142,7 @@
         <v>1.7</v>
       </c>
       <c r="B37" s="129" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D37" s="122"/>
       <c r="E37" s="123"/>
@@ -7376,13 +7376,13 @@
       <c r="BM39" s="108"/>
       <c r="BN39" s="108"/>
     </row>
-    <row r="40" spans="1:66" s="41" customFormat="1" ht="18" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:66" s="41" customFormat="1" ht="26" x14ac:dyDescent="0.15">
       <c r="A40" s="40" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>1.7.3</v>
       </c>
       <c r="B40" s="78" t="s">
-        <v>172</v>
+        <v>194</v>
       </c>
       <c r="D40" s="79"/>
       <c r="E40" s="61">
@@ -7466,7 +7466,7 @@
         <v>1.8</v>
       </c>
       <c r="B41" s="129" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D41" s="122"/>
       <c r="E41" s="123"/>
@@ -7706,7 +7706,7 @@
         <v>1.8.3</v>
       </c>
       <c r="B44" s="78" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D44" s="79"/>
       <c r="E44" s="61">
@@ -7790,7 +7790,7 @@
         <v>1.9</v>
       </c>
       <c r="B45" s="129" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D45" s="122"/>
       <c r="E45" s="123"/>
@@ -8438,7 +8438,7 @@
         <v>1.10.3</v>
       </c>
       <c r="B53" s="78" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D53" s="79"/>
       <c r="E53" s="61">
@@ -8522,7 +8522,7 @@
         <v>1.11</v>
       </c>
       <c r="B54" s="129" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D54" s="122"/>
       <c r="E54" s="123"/>
@@ -8678,7 +8678,7 @@
         <v>1.12.1</v>
       </c>
       <c r="B56" s="78" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D56" s="79"/>
       <c r="E56" s="61">
@@ -8756,13 +8756,13 @@
       <c r="BM56" s="108"/>
       <c r="BN56" s="108"/>
     </row>
-    <row r="57" spans="1:66" s="41" customFormat="1" ht="18" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:66" s="41" customFormat="1" ht="26" x14ac:dyDescent="0.15">
       <c r="A57" s="40" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>1.13</v>
       </c>
       <c r="B57" s="78" t="s">
-        <v>170</v>
+        <v>193</v>
       </c>
       <c r="D57" s="79"/>
       <c r="E57" s="61">
@@ -8846,7 +8846,7 @@
         <v>2</v>
       </c>
       <c r="B58" s="34" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="D58" s="36"/>
       <c r="E58" s="63"/>
@@ -8924,7 +8924,7 @@
         <v>2.1</v>
       </c>
       <c r="B59" s="78" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C59" s="41"/>
       <c r="D59" s="79"/>
@@ -9009,7 +9009,7 @@
         <v>3</v>
       </c>
       <c r="B60" s="34" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="D60" s="36"/>
       <c r="E60" s="63"/>
@@ -9087,7 +9087,7 @@
         <v>3.1</v>
       </c>
       <c r="B61" s="78" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="D61" s="79"/>
       <c r="E61" s="61">
@@ -9171,7 +9171,7 @@
         <v>3.2</v>
       </c>
       <c r="B62" s="78" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D62" s="79"/>
       <c r="E62" s="61">
@@ -9255,7 +9255,7 @@
         <v>3.3</v>
       </c>
       <c r="B63" s="78" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D63" s="79"/>
       <c r="E63" s="61">
@@ -9339,7 +9339,7 @@
         <v>3.4</v>
       </c>
       <c r="B64" s="78" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="D64" s="79"/>
       <c r="E64" s="61">
@@ -9423,7 +9423,7 @@
         <v>3.4.1</v>
       </c>
       <c r="B65" s="78" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="D65" s="79"/>
       <c r="E65" s="61">
@@ -9507,7 +9507,7 @@
         <v>3.5</v>
       </c>
       <c r="B66" s="78" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D66" s="79"/>
       <c r="E66" s="61">
@@ -9591,7 +9591,7 @@
         <v>3.6</v>
       </c>
       <c r="B67" s="78" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="D67" s="79"/>
       <c r="E67" s="61">
@@ -9675,7 +9675,7 @@
         <v>3.7</v>
       </c>
       <c r="B68" s="78" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="D68" s="79"/>
       <c r="E68" s="61">
@@ -9759,7 +9759,7 @@
         <v>4</v>
       </c>
       <c r="B69" s="34" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="D69" s="36"/>
       <c r="E69" s="63"/>
@@ -9837,7 +9837,7 @@
         <v>4.1</v>
       </c>
       <c r="B70" s="78" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="D70" s="79"/>
       <c r="E70" s="61">

</xml_diff>